<commit_message>
Adding code for final graphs
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELIAV\PycharmProjects\FinalProjectRL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E207DD91-F2F2-4C00-A0A2-37F5CA846159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACDAC95-42BD-4747-8121-816C025A3EBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="71">
   <si>
     <t>Light</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>2 (or board_size // 3 in case of dumb light agent)</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>? (200)</t>
@@ -707,97 +704,209 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -809,118 +918,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1205,961 +1202,961 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="16"/>
-    <col min="4" max="4" width="14.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9" style="16"/>
-    <col min="9" max="9" width="14.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="8"/>
+    <col min="4" max="4" width="14.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="8"/>
+    <col min="9" max="9" width="14.125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="53.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="46.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="F1" s="15" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="K1" s="15" t="s">
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="K1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="P1" s="18" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="P1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="49" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="65" t="s">
+      <c r="Q2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="68" t="s">
+      <c r="R2" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="73" t="s">
+      <c r="K3" s="8"/>
+      <c r="L3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="5"/>
-      <c r="Q3" s="59" t="s">
+      <c r="Q3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="60">
+      <c r="R3" s="29">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B4" s="34"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="31" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="31" t="s">
+      <c r="G4" s="50"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="23" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="5"/>
-      <c r="Q4" s="59" t="s">
+      <c r="Q4" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="60">
+      <c r="R4" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="34"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="31" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="31" t="s">
+      <c r="G5" s="50"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="25" t="s">
+      <c r="K5" s="8"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="P5" s="5"/>
-      <c r="Q5" s="59" t="s">
+      <c r="Q5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="R5" s="60">
+      <c r="R5" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B6" s="34"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="32" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="32" t="s">
+      <c r="G6" s="50"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="41" t="s">
+      <c r="K6" s="8"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="16" t="s">
         <v>6</v>
       </c>
       <c r="P6" s="5"/>
-      <c r="Q6" s="59" t="s">
+      <c r="Q6" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="60">
+      <c r="R6" s="29">
         <v>0.97</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="34"/>
-      <c r="C7" s="41" t="s">
+      <c r="B7" s="50"/>
+      <c r="C7" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="44" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="26" t="s">
+      <c r="K7" s="8"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P7" s="5"/>
-      <c r="Q7" s="59" t="s">
+      <c r="Q7" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="60" t="s">
-        <v>67</v>
+      <c r="R7" s="29" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="34"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="26" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="31" t="s">
+      <c r="G8" s="50"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="27" t="s">
+      <c r="K8" s="8"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="P8" s="5"/>
-      <c r="Q8" s="59" t="s">
+      <c r="Q8" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="R8" s="60" t="s">
-        <v>66</v>
+      <c r="R8" s="29" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="34"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="26" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="31" t="s">
+      <c r="G9" s="50"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="38" t="s">
+      <c r="K9" s="8"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="23" t="s">
+      <c r="N9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P9" s="6"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="69"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="38"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="34"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="27" t="s">
+      <c r="B10" s="50"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="32" t="s">
+      <c r="G10" s="50"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="23" t="s">
+      <c r="K10" s="8"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="67" t="s">
+      <c r="Q10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="70" t="s">
+      <c r="R10" s="39" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="8">
         <v>5</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="50"/>
+      <c r="C11" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="44" t="s">
+      <c r="G11" s="50"/>
+      <c r="H11" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L11" s="73"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="46"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P11" s="5"/>
-      <c r="Q11" s="61" t="s">
+      <c r="Q11" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="62" t="s">
+      <c r="R11" s="31" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="8">
         <v>2</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="31" t="s">
+      <c r="B12" s="50"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="8" t="s">
         <v>63</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="50"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="R12" s="29">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>9</v>
+      </c>
+      <c r="B13" s="50"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="R12" s="60">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
-        <v>9</v>
-      </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="31" t="s">
+      <c r="G13" s="50"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="8" t="s">
         <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="46"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="R13" s="29">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>4</v>
+      </c>
+      <c r="B14" s="72"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="73"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="R13" s="60">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
-        <v>4</v>
-      </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="32" t="s">
+      <c r="G14" s="72"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>68</v>
+      <c r="J14" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="73"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="23" t="s">
+      <c r="L14" s="46"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P14" s="6"/>
-      <c r="Q14" s="66" t="s">
+      <c r="Q14" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="R14" s="69">
+      <c r="R14" s="38">
         <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="44" t="s">
+      <c r="H15" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="76" t="s">
+      <c r="L15" s="46"/>
+      <c r="M15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="N15" s="26" t="s">
+      <c r="N15" s="18" t="s">
         <v>6</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q15" s="67" t="s">
+      <c r="Q15" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="R15" s="70" t="s">
+      <c r="R15" s="39" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="34"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="31" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="31" t="s">
+      <c r="G16" s="50"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="26" t="s">
+      <c r="L16" s="46"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P16" s="5"/>
-      <c r="Q16" s="61" t="s">
+      <c r="Q16" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="R16" s="62" t="s">
+      <c r="R16" s="31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="34"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="31" t="s">
+      <c r="B17" s="50"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="31" t="s">
+      <c r="G17" s="50"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="26" t="s">
+      <c r="L17" s="46"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="18" t="s">
         <v>8</v>
       </c>
       <c r="P17" s="6"/>
-      <c r="Q17" s="66" t="s">
+      <c r="Q17" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="R17" s="69">
+      <c r="R17" s="38">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="34"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="32" t="s">
+      <c r="B18" s="50"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="32" t="s">
+      <c r="G18" s="50"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="14" t="s">
+      <c r="L18" s="46"/>
+      <c r="M18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="N18" s="23" t="s">
+      <c r="N18" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q18" s="61" t="s">
+      <c r="Q18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="R18" s="62" t="s">
+      <c r="R18" s="31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="34"/>
-      <c r="C19" s="41" t="s">
+      <c r="B19" s="50"/>
+      <c r="C19" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="44" t="s">
+      <c r="G19" s="50"/>
+      <c r="H19" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="30" t="s">
+      <c r="I19" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="23" t="s">
+      <c r="L19" s="46"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P19" s="5"/>
-      <c r="Q19" s="61" t="s">
+      <c r="Q19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="62" t="s">
+      <c r="R19" s="31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="34"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="26" t="s">
+      <c r="B20" s="50"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="31" t="s">
+      <c r="G20" s="50"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="23" t="s">
+      <c r="L20" s="46"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P20" s="5"/>
-      <c r="Q20" s="59" t="s">
+      <c r="Q20" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="R20" s="60">
+      <c r="R20" s="29">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="34"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="26" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="31" t="s">
+      <c r="G21" s="50"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="73" t="s">
+      <c r="L21" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="N21" s="23" t="s">
+      <c r="N21" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P21" s="5"/>
-      <c r="Q21" s="59" t="s">
+      <c r="Q21" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="60">
+      <c r="R21" s="29">
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="34"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="27" t="s">
+      <c r="B22" s="50"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="32" t="s">
+      <c r="G22" s="50"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="23" t="s">
+      <c r="L22" s="46"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P22" s="5"/>
-      <c r="Q22" s="59" t="s">
+      <c r="Q22" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="R22" s="60">
+      <c r="R22" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="34"/>
-      <c r="C23" s="44" t="s">
+      <c r="B23" s="50"/>
+      <c r="C23" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="44" t="s">
+      <c r="G23" s="50"/>
+      <c r="H23" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="J23" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L23" s="73"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="46"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P23" s="5"/>
-      <c r="Q23" s="59" t="s">
+      <c r="Q23" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="R23" s="60">
+      <c r="R23" s="29">
         <v>1E-3</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="34"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="31" t="s">
+      <c r="B24" s="50"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="8" t="s">
         <v>63</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="46"/>
+      <c r="M24" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="R24" s="29">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B25" s="50"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L24" s="73"/>
-      <c r="M24" s="76" t="s">
-        <v>7</v>
-      </c>
-      <c r="N24" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="R24" s="60">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="34"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="31" t="s">
+      <c r="G25" s="50"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="J25" s="8" t="s">
         <v>62</v>
       </c>
       <c r="K25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25" s="46"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="R25" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="72"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L25" s="73"/>
-      <c r="M25" s="76"/>
-      <c r="N25" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="R25" s="60">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="35"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="32" t="s">
+      <c r="G26" s="72"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" s="35"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>68</v>
+      <c r="J26" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L26" s="73"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="26" t="s">
+      <c r="L26" s="46"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="18" t="s">
         <v>8</v>
       </c>
       <c r="P26" s="2"/>
-      <c r="Q26" s="63" t="s">
+      <c r="Q26" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="R26" s="64">
+      <c r="R26" s="33">
         <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="44" t="s">
+      <c r="H27" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="30" t="s">
+      <c r="I27" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="14" t="s">
+      <c r="L27" s="46"/>
+      <c r="M27" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="23" t="s">
+      <c r="N27" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="34"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="31" t="s">
+      <c r="B28" s="50"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="34"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="31" t="s">
+      <c r="G28" s="50"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="23" t="s">
+      <c r="L28" s="46"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="34"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="31" t="s">
+      <c r="B29" s="50"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="31" t="s">
+      <c r="G29" s="50"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="74"/>
-      <c r="M29" s="77"/>
-      <c r="N29" s="75" t="s">
+      <c r="L29" s="47"/>
+      <c r="M29" s="71"/>
+      <c r="N29" s="42" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="34"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="32" t="s">
+      <c r="B30" s="50"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="34"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="32" t="s">
+      <c r="G30" s="50"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="P30" s="72" t="s">
+      <c r="P30" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="20"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="12"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="34"/>
-      <c r="C31" s="41" t="s">
+      <c r="B31" s="50"/>
+      <c r="C31" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="44" t="s">
+      <c r="G31" s="50"/>
+      <c r="H31" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J31" s="1"/>
@@ -2168,17 +2165,17 @@
         <v>39</v>
       </c>
       <c r="Q31" s="3"/>
-      <c r="R31" s="22"/>
+      <c r="R31" s="14"/>
     </row>
     <row r="32" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="34"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="26" t="s">
+      <c r="B32" s="50"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="31" t="s">
+      <c r="G32" s="50"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J32" s="1"/>
@@ -2187,195 +2184,195 @@
       <c r="Q32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R32" s="22" t="s">
+      <c r="R32" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B33" s="34"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="26" t="s">
+      <c r="B33" s="50"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="31" t="s">
+      <c r="G33" s="50"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="50" t="s">
+      <c r="L33" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="M33" s="51"/>
-      <c r="N33" s="52"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="58"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R33" s="22" t="s">
+      <c r="R33" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B34" s="34"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="27" t="s">
+      <c r="B34" s="50"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="32" t="s">
+      <c r="G34" s="50"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="53"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="61"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R34" s="22" t="s">
+      <c r="R34" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="34"/>
-      <c r="C35" s="44" t="s">
+      <c r="B35" s="50"/>
+      <c r="C35" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G35" s="34"/>
-      <c r="H35" s="44" t="s">
+      <c r="G35" s="50"/>
+      <c r="H35" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="30" t="s">
+      <c r="I35" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="J35" s="16" t="s">
+      <c r="J35" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L35" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L35" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="M35" s="11"/>
-      <c r="N35" s="54"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="64"/>
       <c r="P35" s="5" t="s">
         <v>40</v>
       </c>
       <c r="Q35" s="3"/>
-      <c r="R35" s="22"/>
+      <c r="R35" s="14"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B36" s="34"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="31" t="s">
+      <c r="B36" s="50"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="8" t="s">
         <v>63</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" s="34"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="50"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J36" s="16" t="s">
+      <c r="J36" s="8" t="s">
         <v>63</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="54"/>
+        <v>68</v>
+      </c>
+      <c r="L36" s="62"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="64"/>
       <c r="P36" s="5" t="s">
         <v>41</v>
       </c>
       <c r="Q36" s="3"/>
-      <c r="R36" s="22"/>
+      <c r="R36" s="14"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B37" s="34"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="31" t="s">
+      <c r="B37" s="50"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>71</v>
+      <c r="E37" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G37" s="34"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="31" t="s">
+      <c r="G37" s="50"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="8" t="s">
         <v>62</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L37" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L37" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="12"/>
-      <c r="N37" s="55"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="67"/>
       <c r="P37" s="5" t="s">
         <v>48</v>
       </c>
       <c r="Q37" s="3"/>
-      <c r="R37" s="22"/>
+      <c r="R37" s="14"/>
     </row>
     <row r="38" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="37"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="33" t="s">
+      <c r="B38" s="51"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>68</v>
+      <c r="E38" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G38" s="37"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" s="51"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J38" s="16" t="s">
-        <v>68</v>
+      <c r="J38" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="56"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="58"/>
-      <c r="P38" s="71"/>
-      <c r="Q38" s="28" t="s">
+      <c r="L38" s="68"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="70"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="R38" s="29" t="s">
+      <c r="R38" s="21" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2393,7 +2390,7 @@
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.2">
       <c r="J42" s="1"/>
-      <c r="P42" s="78"/>
+      <c r="P42" s="43"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.2">
       <c r="J43" s="1"/>
@@ -2406,11 +2403,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="L3:L11"/>
-    <mergeCell ref="L12:L20"/>
-    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="B3:B14"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="B27:B38"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="G15:G26"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="H23:H26"/>
     <mergeCell ref="M21:M23"/>
     <mergeCell ref="M24:M26"/>
     <mergeCell ref="L21:L29"/>
@@ -2427,26 +2439,11 @@
     <mergeCell ref="G3:G14"/>
     <mergeCell ref="H3:H6"/>
     <mergeCell ref="H7:H10"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="G15:G26"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="B3:B14"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="B27:B38"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="L3:L11"/>
+    <mergeCell ref="L12:L20"/>
+    <mergeCell ref="M18:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
setting up training of mcts
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELIAV\PycharmProjects\FinalProjectRL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACDAC95-42BD-4747-8121-816C025A3EBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80BA01B-F702-4099-9EE8-345AC8663B49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="71">
   <si>
     <t>Light</t>
   </si>
@@ -198,9 +198,6 @@
     <t>epochs</t>
   </si>
   <si>
-    <t>0.5, 1, 1.5, 2</t>
-  </si>
-  <si>
     <t>gamma</t>
   </si>
   <si>
@@ -231,13 +228,16 @@
     <t>Laptop</t>
   </si>
   <si>
-    <t>Done, Running</t>
-  </si>
-  <si>
     <t>Done, Done</t>
   </si>
   <si>
     <t>Windows,Linux Server</t>
+  </si>
+  <si>
+    <t>0.5, 1, 1.5</t>
+  </si>
+  <si>
+    <t>Running, Running</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -767,6 +767,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -849,15 +852,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -916,6 +910,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1202,7 +1205,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1215,7 +1218,7 @@
     <col min="7" max="8" width="9" style="8"/>
     <col min="9" max="9" width="14.125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="28.125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="46.5" bestFit="1" customWidth="1"/>
@@ -1225,19 +1228,19 @@
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
       <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="K1" s="7" t="s">
         <v>14</v>
       </c>
@@ -1286,229 +1289,244 @@
       <c r="P2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="Q2" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="37" t="s">
-        <v>64</v>
+      <c r="R2" s="38" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="28" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="8"/>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="74" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="5"/>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="29">
+      <c r="R3" s="30">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B4" s="50"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="23" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="23" t="s">
+      <c r="G4" s="51"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="28" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="8"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="77"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="75"/>
       <c r="N4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="5"/>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="29">
+      <c r="R4" s="30">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="23" t="s">
+      <c r="G5" s="51"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="28" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="8"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="78"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="76"/>
       <c r="N5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="P5" s="5"/>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="R5" s="29">
+      <c r="R5" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B6" s="50"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="24" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="24" t="s">
+      <c r="G6" s="51"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="17" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="73" t="s">
+      <c r="L6" s="47"/>
+      <c r="M6" s="71" t="s">
         <v>7</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>6</v>
       </c>
       <c r="P6" s="5"/>
-      <c r="Q6" s="28" t="s">
+      <c r="Q6" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="29">
+      <c r="R6" s="30">
         <v>0.97</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="50"/>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="71" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="52" t="s">
+      <c r="G7" s="51"/>
+      <c r="H7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="74"/>
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" s="47"/>
+      <c r="M7" s="72"/>
       <c r="N7" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P7" s="5"/>
-      <c r="Q7" s="28" t="s">
+      <c r="Q7" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="29" t="s">
-        <v>66</v>
+      <c r="R7" s="30" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="50"/>
-      <c r="C8" s="74"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="23" t="s">
+      <c r="G8" s="51"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="75"/>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="47"/>
+      <c r="M8" s="73"/>
       <c r="N8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="P8" s="5"/>
-      <c r="Q8" s="28" t="s">
+      <c r="Q8" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="R8" s="29" t="s">
-        <v>65</v>
+      <c r="R8" s="30" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="50"/>
-      <c r="C9" s="74"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="23" t="s">
+      <c r="G9" s="51"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="76" t="s">
+      <c r="J9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="47"/>
+      <c r="M9" s="74" t="s">
         <v>8</v>
       </c>
       <c r="N9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P9" s="6"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="38"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="39"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="50"/>
-      <c r="C10" s="75"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="24" t="s">
+      <c r="G10" s="51"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="77"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="75"/>
       <c r="N10" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="36" t="s">
+      <c r="Q10" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="39" t="s">
+      <c r="R10" s="40" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1516,85 +1534,85 @@
       <c r="A11" s="8">
         <v>5</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="52" t="s">
+      <c r="B11" s="51"/>
+      <c r="C11" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="51"/>
+      <c r="H11" s="53" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="46"/>
-      <c r="M11" s="77"/>
+        <v>67</v>
+      </c>
+      <c r="L11" s="47"/>
+      <c r="M11" s="75"/>
       <c r="N11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P11" s="5"/>
-      <c r="Q11" s="30" t="s">
+      <c r="Q11" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="31" t="s">
-        <v>60</v>
+      <c r="R11" s="32" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>2</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="53"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="50"/>
-      <c r="H12" s="53"/>
+        <v>67</v>
+      </c>
+      <c r="G12" s="51"/>
+      <c r="H12" s="54"/>
       <c r="I12" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="M12" s="44" t="s">
+      <c r="M12" s="45" t="s">
         <v>6</v>
       </c>
       <c r="N12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P12" s="5"/>
-      <c r="Q12" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="R12" s="29">
+      <c r="Q12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="R12" s="30">
         <v>0.99</v>
       </c>
     </row>
@@ -1602,38 +1620,38 @@
       <c r="A13" s="8">
         <v>9</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="53"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="50"/>
-      <c r="H13" s="53"/>
+        <v>67</v>
+      </c>
+      <c r="G13" s="51"/>
+      <c r="H13" s="54"/>
       <c r="I13" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L13" s="46"/>
-      <c r="M13" s="44"/>
+        <v>67</v>
+      </c>
+      <c r="L13" s="47"/>
+      <c r="M13" s="45"/>
       <c r="N13" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P13" s="5"/>
-      <c r="Q13" s="28" t="s">
+      <c r="Q13" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="R13" s="29">
+      <c r="R13" s="30">
         <v>1E-3</v>
       </c>
     </row>
@@ -1641,64 +1659,64 @@
       <c r="A14" s="8">
         <v>4</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="54"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="72"/>
-      <c r="H14" s="54"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="55"/>
       <c r="I14" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L14" s="46"/>
-      <c r="M14" s="44"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="45"/>
       <c r="N14" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P14" s="6"/>
-      <c r="Q14" s="35" t="s">
+      <c r="Q14" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="R14" s="38">
+      <c r="R14" s="39">
         <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="13" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="45" t="s">
+      <c r="L15" s="47"/>
+      <c r="M15" s="46" t="s">
         <v>7</v>
       </c>
       <c r="N15" s="18" t="s">
@@ -1707,80 +1725,80 @@
       <c r="P15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q15" s="36" t="s">
+      <c r="Q15" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="R15" s="39" t="s">
+      <c r="R15" s="40" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="50"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="23" t="s">
+      <c r="B16" s="51"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="23" t="s">
+      <c r="G16" s="51"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="28" t="s">
         <v>10</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="45"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="46"/>
       <c r="N16" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P16" s="5"/>
-      <c r="Q16" s="30" t="s">
+      <c r="Q16" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="R16" s="31" t="s">
-        <v>57</v>
+      <c r="R16" s="32" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="50"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="23" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="23" t="s">
+      <c r="G17" s="51"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="28" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="45"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="46"/>
       <c r="N17" s="18" t="s">
         <v>8</v>
       </c>
       <c r="P17" s="6"/>
-      <c r="Q17" s="35" t="s">
+      <c r="Q17" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="R17" s="38">
+      <c r="R17" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="50"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="24" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="50"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="24" t="s">
+      <c r="G18" s="51"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="44" t="s">
+      <c r="L18" s="47"/>
+      <c r="M18" s="45" t="s">
         <v>8</v>
       </c>
       <c r="N18" s="15" t="s">
@@ -1789,298 +1807,310 @@
       <c r="P18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q18" s="30" t="s">
+      <c r="Q18" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="R18" s="31" t="s">
+      <c r="R18" s="32" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="50"/>
-      <c r="C19" s="73" t="s">
+      <c r="B19" s="51"/>
+      <c r="C19" s="71" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="50"/>
-      <c r="H19" s="52" t="s">
+      <c r="G19" s="51"/>
+      <c r="H19" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="44"/>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="47"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P19" s="5"/>
-      <c r="Q19" s="30" t="s">
+      <c r="Q19" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="31" t="s">
-        <v>57</v>
+      <c r="R19" s="32" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="50"/>
-      <c r="C20" s="74"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="50"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="23" t="s">
+      <c r="G20" s="51"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="44"/>
+      <c r="J20" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="47"/>
+      <c r="M20" s="45"/>
       <c r="N20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P20" s="5"/>
-      <c r="Q20" s="28" t="s">
+      <c r="Q20" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="R20" s="29">
+      <c r="R20" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="50"/>
-      <c r="C21" s="74"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="50"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="23" t="s">
+      <c r="G21" s="51"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="46" t="s">
+      <c r="J21" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="44" t="s">
+      <c r="M21" s="45" t="s">
         <v>6</v>
       </c>
       <c r="N21" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P21" s="5"/>
-      <c r="Q21" s="28" t="s">
+      <c r="Q21" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="29">
+      <c r="R21" s="30">
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="50"/>
-      <c r="C22" s="75"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="73"/>
       <c r="D22" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="50"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="24" t="s">
+      <c r="G22" s="51"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="44"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="45"/>
       <c r="N22" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P22" s="5"/>
-      <c r="Q22" s="28" t="s">
+      <c r="Q22" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="R22" s="29">
+      <c r="R22" s="30">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="50"/>
-      <c r="C23" s="52" t="s">
+      <c r="B23" s="51"/>
+      <c r="C23" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="50"/>
-      <c r="H23" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="51"/>
+      <c r="H23" s="53" t="s">
         <v>8</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L23" s="46"/>
-      <c r="M23" s="44"/>
+        <v>67</v>
+      </c>
+      <c r="L23" s="47"/>
+      <c r="M23" s="45"/>
       <c r="N23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P23" s="5"/>
-      <c r="Q23" s="28" t="s">
+      <c r="Q23" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="R23" s="29">
+      <c r="R23" s="30">
         <v>1E-3</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="50"/>
-      <c r="C24" s="53"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="50"/>
-      <c r="H24" s="53"/>
+        <v>67</v>
+      </c>
+      <c r="G24" s="51"/>
+      <c r="H24" s="54"/>
       <c r="I24" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L24" s="46"/>
-      <c r="M24" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="L24" s="47"/>
+      <c r="M24" s="46" t="s">
         <v>7</v>
       </c>
       <c r="N24" s="18" t="s">
         <v>6</v>
       </c>
       <c r="P24" s="5"/>
-      <c r="Q24" s="28" t="s">
+      <c r="Q24" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="R24" s="29">
+      <c r="R24" s="30">
         <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="50"/>
-      <c r="C25" s="53"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="54"/>
       <c r="D25" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="50"/>
-      <c r="H25" s="53"/>
+        <v>67</v>
+      </c>
+      <c r="G25" s="51"/>
+      <c r="H25" s="54"/>
       <c r="I25" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L25" s="46"/>
-      <c r="M25" s="45"/>
+        <v>67</v>
+      </c>
+      <c r="L25" s="47"/>
+      <c r="M25" s="46"/>
       <c r="N25" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P25" s="5"/>
-      <c r="Q25" s="28" t="s">
+      <c r="Q25" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="R25" s="29">
+      <c r="R25" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="72"/>
-      <c r="C26" s="54"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="55"/>
       <c r="D26" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="72"/>
-      <c r="H26" s="54"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="55"/>
       <c r="I26" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J26" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L26" s="46"/>
-      <c r="M26" s="45"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="46"/>
       <c r="N26" s="18" t="s">
         <v>8</v>
       </c>
       <c r="P26" s="2"/>
-      <c r="Q26" s="32" t="s">
+      <c r="Q26" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="R26" s="33">
+      <c r="R26" s="34">
         <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="49" t="s">
+      <c r="G27" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="52" t="s">
+      <c r="H27" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="13" t="s">
         <v>9</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="44" t="s">
+      <c r="L27" s="47"/>
+      <c r="M27" s="45" t="s">
         <v>8</v>
       </c>
       <c r="N27" s="15" t="s">
@@ -2088,79 +2118,83 @@
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="50"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="23" t="s">
+      <c r="B28" s="51"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="50"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="23" t="s">
+      <c r="G28" s="51"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="28" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="44"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="45"/>
       <c r="N28" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="23" t="s">
+      <c r="B29" s="51"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="50"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="23" t="s">
+      <c r="G29" s="51"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="28" t="s">
         <v>11</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="71"/>
-      <c r="N29" s="42" t="s">
+      <c r="L29" s="48"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="43" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="24" t="s">
+      <c r="B30" s="51"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="50"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="24" t="s">
+      <c r="G30" s="51"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="P30" s="41" t="s">
+      <c r="P30" s="42" t="s">
         <v>38</v>
       </c>
       <c r="Q30" s="11"/>
       <c r="R30" s="12"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="50"/>
-      <c r="C31" s="73" t="s">
+      <c r="B31" s="51"/>
+      <c r="C31" s="71" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="50"/>
-      <c r="H31" s="52" t="s">
+      <c r="G31" s="51"/>
+      <c r="H31" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="22" t="s">
+      <c r="I31" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="J31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="P31" s="5" t="s">
         <v>39</v>
       </c>
@@ -2168,18 +2202,22 @@
       <c r="R31" s="14"/>
     </row>
     <row r="32" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="50"/>
-      <c r="C32" s="74"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="72"/>
       <c r="D32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="50"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="23" t="s">
+      <c r="G32" s="51"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+      <c r="J32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="3" t="s">
         <v>44</v>
@@ -2189,23 +2227,27 @@
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B33" s="50"/>
-      <c r="C33" s="74"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="72"/>
       <c r="D33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="50"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="23" t="s">
+      <c r="G33" s="51"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="M33" s="57"/>
-      <c r="N33" s="58"/>
+      <c r="J33" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L33" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" s="78"/>
+      <c r="N33" s="79"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="3" t="s">
         <v>43</v>
@@ -2215,21 +2257,21 @@
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B34" s="50"/>
-      <c r="C34" s="75"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="73"/>
       <c r="D34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="50"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="24" t="s">
+      <c r="G34" s="51"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="61"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="62"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="3" t="s">
         <v>45</v>
@@ -2239,37 +2281,37 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="50"/>
-      <c r="C35" s="52" t="s">
+      <c r="B35" s="51"/>
+      <c r="C35" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="50"/>
-      <c r="H35" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="51"/>
+      <c r="H35" s="53" t="s">
         <v>8</v>
       </c>
       <c r="I35" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L35" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M35" s="63"/>
-      <c r="N35" s="64"/>
+        <v>67</v>
+      </c>
+      <c r="L35" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="M35" s="58"/>
+      <c r="N35" s="59"/>
       <c r="P35" s="5" t="s">
         <v>40</v>
       </c>
@@ -2277,31 +2319,31 @@
       <c r="R35" s="14"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B36" s="50"/>
-      <c r="C36" s="53"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G36" s="50"/>
-      <c r="H36" s="53"/>
+        <v>67</v>
+      </c>
+      <c r="G36" s="51"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L36" s="62"/>
-      <c r="M36" s="63"/>
-      <c r="N36" s="64"/>
+        <v>67</v>
+      </c>
+      <c r="L36" s="57"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="59"/>
       <c r="P36" s="5" t="s">
         <v>41</v>
       </c>
@@ -2309,33 +2351,33 @@
       <c r="R36" s="14"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B37" s="50"/>
-      <c r="C37" s="53"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" s="50"/>
-      <c r="H37" s="53"/>
+        <v>67</v>
+      </c>
+      <c r="G37" s="51"/>
+      <c r="H37" s="54"/>
       <c r="I37" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L37" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="L37" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="66"/>
-      <c r="N37" s="67"/>
+      <c r="M37" s="64"/>
+      <c r="N37" s="65"/>
       <c r="P37" s="5" t="s">
         <v>48</v>
       </c>
@@ -2343,37 +2385,37 @@
       <c r="R37" s="14"/>
     </row>
     <row r="38" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="51"/>
-      <c r="C38" s="55"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="56"/>
       <c r="D38" s="25" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G38" s="51"/>
-      <c r="H38" s="55"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="56"/>
       <c r="I38" s="25" t="s">
         <v>12</v>
       </c>
       <c r="J38" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L38" s="68"/>
-      <c r="M38" s="69"/>
-      <c r="N38" s="70"/>
-      <c r="P38" s="40"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="68"/>
+      <c r="P38" s="41"/>
       <c r="Q38" s="20" t="s">
         <v>49</v>
       </c>
       <c r="R38" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
@@ -2390,7 +2432,7 @@
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.2">
       <c r="J42" s="1"/>
-      <c r="P42" s="43"/>
+      <c r="P42" s="44"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.2">
       <c r="J43" s="1"/>

</xml_diff>

<commit_message>
Rearranging the /docs partition
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELIAV\PycharmProjects\FinalProjectRL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80BA01B-F702-4099-9EE8-345AC8663B49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A9F0A0-DFBA-4AC6-9E6E-B7ECD65441B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1205,7 +1205,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="M21" sqref="M21:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
All set up and is Ready to train the AlphaZero Agent!!
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELIAV\PycharmProjects\FinalProjectRL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A9F0A0-DFBA-4AC6-9E6E-B7ECD65441B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5954D1-CC69-49B8-8ED0-D086EB1ED57C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="73">
   <si>
     <t>Light</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Parameters meaning</t>
   </si>
   <si>
-    <t>20, 50, 100</t>
-  </si>
-  <si>
     <t>number of episodes per learning</t>
   </si>
   <si>
@@ -238,6 +235,15 @@
   </si>
   <si>
     <t>Running, Running</t>
+  </si>
+  <si>
+    <t>15, 30, 45</t>
+  </si>
+  <si>
+    <t>1.2, 1.4, 1.6</t>
+  </si>
+  <si>
+    <t>5, 10, 15</t>
   </si>
 </sst>
 </file>
@@ -816,6 +822,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,25 +879,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -861,15 +906,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -889,36 +925,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1205,7 +1211,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21:M23"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1228,19 +1234,19 @@
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
       <c r="K1" s="7" t="s">
         <v>14</v>
       </c>
@@ -1293,33 +1299,38 @@
         <v>32</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="49" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="50" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="47" t="s">
+      <c r="J3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="74" t="s">
+      <c r="M3" s="49" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="13" t="s">
@@ -1334,19 +1345,24 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B4" s="51"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="75"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="75"/>
+      <c r="J4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="61"/>
+      <c r="M4" s="50"/>
       <c r="N4" s="15" t="s">
         <v>7</v>
       </c>
@@ -1359,19 +1375,19 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="51"/>
-      <c r="C5" s="75"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="75"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="28" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="8"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="51"/>
       <c r="N5" s="17" t="s">
         <v>8</v>
       </c>
@@ -1384,19 +1400,19 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B6" s="51"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="76"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="17" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="71" t="s">
+      <c r="L6" s="61"/>
+      <c r="M6" s="52" t="s">
         <v>7</v>
       </c>
       <c r="N6" s="16" t="s">
@@ -1411,28 +1427,22 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="51"/>
-      <c r="C7" s="71" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="51"/>
-      <c r="H7" s="74" t="s">
+      <c r="G7" s="45"/>
+      <c r="H7" s="49" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="47"/>
-      <c r="M7" s="72"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="53"/>
       <c r="N7" s="18" t="s">
         <v>7</v>
       </c>
@@ -1441,28 +1451,22 @@
         <v>37</v>
       </c>
       <c r="R7" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="51"/>
-      <c r="C8" s="72"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="51"/>
-      <c r="H8" s="75"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="50"/>
       <c r="I8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="47"/>
-      <c r="M8" s="73"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="54"/>
       <c r="N8" s="19" t="s">
         <v>8</v>
       </c>
@@ -1471,28 +1475,23 @@
         <v>33</v>
       </c>
       <c r="R8" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="51"/>
-      <c r="C9" s="72"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="51"/>
-      <c r="H9" s="75"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="50"/>
       <c r="I9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="47"/>
-      <c r="M9" s="74" t="s">
+      <c r="K9" s="8"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="49" t="s">
         <v>8</v>
       </c>
       <c r="N9" s="15" t="s">
@@ -1503,20 +1502,20 @@
       <c r="R9" s="39"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="51"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="51"/>
-      <c r="H10" s="76"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="75"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="50"/>
       <c r="N10" s="15" t="s">
         <v>7</v>
       </c>
@@ -1532,36 +1531,36 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
-        <v>5</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="45"/>
+      <c r="C11" s="55" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="51"/>
-      <c r="H11" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="45"/>
+      <c r="H11" s="55" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L11" s="47"/>
-      <c r="M11" s="75"/>
+        <v>66</v>
+      </c>
+      <c r="L11" s="61"/>
+      <c r="M11" s="50"/>
       <c r="N11" s="15" t="s">
         <v>8</v>
       </c>
@@ -1570,39 +1569,39 @@
         <v>19</v>
       </c>
       <c r="R11" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
-        <v>2</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="54"/>
+        <v>1</v>
+      </c>
+      <c r="B12" s="45"/>
+      <c r="C12" s="56"/>
       <c r="D12" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="54"/>
+        <v>66</v>
+      </c>
+      <c r="G12" s="45"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="M12" s="45" t="s">
+      <c r="M12" s="59" t="s">
         <v>6</v>
       </c>
       <c r="N12" s="15" t="s">
@@ -1610,7 +1609,7 @@
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R12" s="30">
         <v>0.99</v>
@@ -1618,38 +1617,38 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
-        <v>9</v>
-      </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="54"/>
+        <v>5</v>
+      </c>
+      <c r="B13" s="45"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="54"/>
+        <v>66</v>
+      </c>
+      <c r="G13" s="45"/>
+      <c r="H13" s="56"/>
       <c r="I13" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="47"/>
-      <c r="M13" s="45"/>
+        <v>66</v>
+      </c>
+      <c r="L13" s="61"/>
+      <c r="M13" s="59"/>
       <c r="N13" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P13" s="5"/>
       <c r="Q13" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R13" s="30">
         <v>1E-3</v>
@@ -1657,32 +1656,32 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
-        <v>4</v>
-      </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="55"/>
+        <v>2</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="70"/>
-      <c r="H14" s="55"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="57"/>
       <c r="I14" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="45"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="59"/>
       <c r="N14" s="15" t="s">
         <v>8</v>
       </c>
@@ -1695,28 +1694,32 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="49" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="50" t="s">
+      <c r="G15" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="74" t="s">
+      <c r="H15" s="49" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="46" t="s">
+      <c r="J15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="61"/>
+      <c r="M15" s="60" t="s">
         <v>7</v>
       </c>
       <c r="N15" s="18" t="s">
@@ -1729,24 +1732,28 @@
         <v>20</v>
       </c>
       <c r="R15" s="40" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="51"/>
-      <c r="C16" s="75"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="75"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="46"/>
+      <c r="J16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="61"/>
+      <c r="M16" s="60"/>
       <c r="N16" s="18" t="s">
         <v>7</v>
       </c>
@@ -1755,24 +1762,24 @@
         <v>22</v>
       </c>
       <c r="R16" s="32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="51"/>
-      <c r="C17" s="75"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="75"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="28" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="46"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="60"/>
       <c r="N17" s="18" t="s">
         <v>8</v>
       </c>
@@ -1781,24 +1788,24 @@
         <v>21</v>
       </c>
       <c r="R17" s="39">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="51"/>
-      <c r="C18" s="76"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="76"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="45" t="s">
+      <c r="L18" s="61"/>
+      <c r="M18" s="59" t="s">
         <v>8</v>
       </c>
       <c r="N18" s="15" t="s">
@@ -1811,32 +1818,28 @@
         <v>23</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="51"/>
-      <c r="C19" s="71" t="s">
+      <c r="B19" s="45"/>
+      <c r="C19" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="51"/>
-      <c r="H19" s="74" t="s">
+      <c r="G19" s="45"/>
+      <c r="H19" s="49" t="s">
         <v>7</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J19" t="s">
-        <v>61</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L19" s="47"/>
-      <c r="M19" s="45"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="59"/>
       <c r="N19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1845,28 +1848,24 @@
         <v>22</v>
       </c>
       <c r="R19" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="51"/>
-      <c r="C20" s="72"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="51"/>
-      <c r="H20" s="75"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J20" t="s">
-        <v>62</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="47"/>
-      <c r="M20" s="45"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="59"/>
       <c r="N20" s="15" t="s">
         <v>8</v>
       </c>
@@ -1875,30 +1874,25 @@
         <v>24</v>
       </c>
       <c r="R20" s="30">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="51"/>
-      <c r="C21" s="72"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="75"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="50"/>
       <c r="I21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J21" t="s">
-        <v>60</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="47" t="s">
+      <c r="K21" s="8"/>
+      <c r="L21" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="45" t="s">
+      <c r="M21" s="59" t="s">
         <v>6</v>
       </c>
       <c r="N21" s="15" t="s">
@@ -1913,96 +1907,96 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="51"/>
-      <c r="C22" s="73"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="54"/>
       <c r="D22" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="51"/>
-      <c r="H22" s="76"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="45"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="59"/>
       <c r="N22" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P22" s="5"/>
       <c r="Q22" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R22" s="30">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="51"/>
-      <c r="C23" s="53" t="s">
+      <c r="B23" s="45"/>
+      <c r="C23" s="55" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="51"/>
-      <c r="H23" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="45"/>
+      <c r="H23" s="55" t="s">
         <v>8</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L23" s="47"/>
-      <c r="M23" s="45"/>
+        <v>66</v>
+      </c>
+      <c r="L23" s="61"/>
+      <c r="M23" s="59"/>
       <c r="N23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R23" s="30">
         <v>1E-3</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="51"/>
-      <c r="C24" s="54"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="51"/>
-      <c r="H24" s="54"/>
+        <v>66</v>
+      </c>
+      <c r="G24" s="45"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L24" s="47"/>
-      <c r="M24" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="61"/>
+      <c r="M24" s="60" t="s">
         <v>7</v>
       </c>
       <c r="N24" s="18" t="s">
@@ -2010,73 +2004,73 @@
       </c>
       <c r="P24" s="5"/>
       <c r="Q24" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R24" s="30">
         <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="51"/>
-      <c r="C25" s="54"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" s="51"/>
-      <c r="H25" s="54"/>
+        <v>66</v>
+      </c>
+      <c r="G25" s="45"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L25" s="47"/>
-      <c r="M25" s="46"/>
+        <v>66</v>
+      </c>
+      <c r="L25" s="61"/>
+      <c r="M25" s="60"/>
       <c r="N25" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R25" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="70"/>
-      <c r="C26" s="55"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" s="70"/>
-      <c r="H26" s="55"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="57"/>
       <c r="I26" s="24" t="s">
         <v>12</v>
       </c>
       <c r="J26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" s="47"/>
-      <c r="M26" s="46"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="60"/>
       <c r="N26" s="18" t="s">
         <v>8</v>
       </c>
@@ -2089,28 +2083,32 @@
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="74" t="s">
+      <c r="C27" s="49" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="74" t="s">
+      <c r="H27" s="49" t="s">
         <v>6</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="45" t="s">
+      <c r="J27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27" s="61"/>
+      <c r="M27" s="59" t="s">
         <v>8</v>
       </c>
       <c r="N27" s="15" t="s">
@@ -2118,51 +2116,55 @@
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="51"/>
-      <c r="C28" s="75"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="51"/>
-      <c r="H28" s="75"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="50"/>
       <c r="I28" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="45"/>
+      <c r="J28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L28" s="61"/>
+      <c r="M28" s="59"/>
       <c r="N28" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="51"/>
-      <c r="C29" s="75"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="51"/>
-      <c r="H29" s="75"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="50"/>
       <c r="I29" s="28" t="s">
         <v>11</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="69"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="79"/>
       <c r="N29" s="43" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="51"/>
-      <c r="C30" s="76"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="51"/>
-      <c r="H30" s="76"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="51"/>
       <c r="I30" s="17" t="s">
         <v>12</v>
       </c>
@@ -2175,26 +2177,22 @@
       <c r="R30" s="12"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="51"/>
-      <c r="C31" s="71" t="s">
+      <c r="B31" s="45"/>
+      <c r="C31" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="51"/>
-      <c r="H31" s="74" t="s">
+      <c r="G31" s="45"/>
+      <c r="H31" s="49" t="s">
         <v>7</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J31" t="s">
-        <v>61</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="1"/>
       <c r="P31" s="5" t="s">
         <v>39</v>
       </c>
@@ -2202,22 +2200,18 @@
       <c r="R31" s="14"/>
     </row>
     <row r="32" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="51"/>
-      <c r="C32" s="72"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="51"/>
-      <c r="H32" s="75"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="50"/>
       <c r="I32" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="J32" s="8"/>
+      <c r="K32" s="1"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="3" t="s">
         <v>44</v>
@@ -2227,27 +2221,22 @@
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B33" s="51"/>
-      <c r="C33" s="72"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="51"/>
-      <c r="H33" s="75"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="50"/>
       <c r="I33" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J33" t="s">
-        <v>60</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="77" t="s">
+      <c r="K33" s="8"/>
+      <c r="L33" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="78"/>
-      <c r="N33" s="79"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="66"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="3" t="s">
         <v>43</v>
@@ -2257,21 +2246,21 @@
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B34" s="51"/>
-      <c r="C34" s="73"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="51"/>
-      <c r="H34" s="76"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="62"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="69"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="3" t="s">
         <v>45</v>
@@ -2281,37 +2270,37 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="51"/>
-      <c r="C35" s="53" t="s">
+      <c r="B35" s="45"/>
+      <c r="C35" s="55" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="51"/>
-      <c r="H35" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="45"/>
+      <c r="H35" s="55" t="s">
         <v>8</v>
       </c>
       <c r="I35" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L35" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="L35" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="M35" s="58"/>
-      <c r="N35" s="59"/>
+      <c r="M35" s="71"/>
+      <c r="N35" s="72"/>
       <c r="P35" s="5" t="s">
         <v>40</v>
       </c>
@@ -2319,31 +2308,31 @@
       <c r="R35" s="14"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B36" s="51"/>
-      <c r="C36" s="54"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="56"/>
       <c r="D36" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" s="51"/>
-      <c r="H36" s="54"/>
+        <v>66</v>
+      </c>
+      <c r="G36" s="45"/>
+      <c r="H36" s="56"/>
       <c r="I36" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L36" s="57"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="59"/>
+        <v>66</v>
+      </c>
+      <c r="L36" s="70"/>
+      <c r="M36" s="71"/>
+      <c r="N36" s="72"/>
       <c r="P36" s="5" t="s">
         <v>41</v>
       </c>
@@ -2351,33 +2340,33 @@
       <c r="R36" s="14"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B37" s="51"/>
-      <c r="C37" s="54"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="56"/>
       <c r="D37" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G37" s="51"/>
-      <c r="H37" s="54"/>
+        <v>66</v>
+      </c>
+      <c r="G37" s="45"/>
+      <c r="H37" s="56"/>
       <c r="I37" s="23" t="s">
         <v>11</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L37" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="L37" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="64"/>
-      <c r="N37" s="65"/>
+      <c r="M37" s="74"/>
+      <c r="N37" s="75"/>
       <c r="P37" s="5" t="s">
         <v>48</v>
       </c>
@@ -2385,37 +2374,37 @@
       <c r="R37" s="14"/>
     </row>
     <row r="38" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="52"/>
-      <c r="C38" s="56"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="58"/>
       <c r="D38" s="25" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" s="52"/>
-      <c r="H38" s="56"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="58"/>
       <c r="I38" s="25" t="s">
         <v>12</v>
       </c>
       <c r="J38" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L38" s="66"/>
-      <c r="M38" s="67"/>
-      <c r="N38" s="68"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="77"/>
+      <c r="N38" s="78"/>
       <c r="P38" s="41"/>
       <c r="Q38" s="20" t="s">
         <v>49</v>
       </c>
       <c r="R38" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
@@ -2445,6 +2434,35 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="L33:N34"/>
+    <mergeCell ref="L35:N36"/>
+    <mergeCell ref="L37:N38"/>
+    <mergeCell ref="M27:M29"/>
+    <mergeCell ref="G3:G14"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="L3:L11"/>
+    <mergeCell ref="L12:L20"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G27:G38"/>
+    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="G15:G26"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="M21:M23"/>
+    <mergeCell ref="M24:M26"/>
+    <mergeCell ref="L21:L29"/>
     <mergeCell ref="B3:B14"/>
     <mergeCell ref="B15:B26"/>
     <mergeCell ref="B27:B38"/>
@@ -2457,37 +2475,11 @@
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="C31:C34"/>
     <mergeCell ref="C35:C38"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="G15:G26"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="M21:M23"/>
-    <mergeCell ref="M24:M26"/>
-    <mergeCell ref="L21:L29"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G27:G38"/>
-    <mergeCell ref="H27:H30"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="L33:N34"/>
-    <mergeCell ref="L35:N36"/>
-    <mergeCell ref="L37:N38"/>
-    <mergeCell ref="M27:M29"/>
-    <mergeCell ref="G3:G14"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="L3:L11"/>
-    <mergeCell ref="L12:L20"/>
-    <mergeCell ref="M18:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="R18" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update project report and add alphazero evaluation results
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELIAV\PycharmProjects\FinalProjectRL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC792733-7B14-4A14-89FC-8C41D280A9C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C40B37-5851-4D27-BF1D-A99C04F25AAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="best configurations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="88">
   <si>
     <t>Light</t>
   </si>
@@ -254,6 +254,42 @@
   </si>
   <si>
     <t>end - 22/4/2021</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>best configurations:</t>
+  </si>
+  <si>
+    <t>first param:</t>
+  </si>
+  <si>
+    <t>Memory Size</t>
+  </si>
+  <si>
+    <t>second param</t>
+  </si>
+  <si>
+    <t>Traget Update</t>
+  </si>
+  <si>
+    <t>Cpuct</t>
+  </si>
+  <si>
+    <t>Monte Carlo Searches</t>
+  </si>
+  <si>
+    <t>first param</t>
+  </si>
+  <si>
+    <t>As zombie</t>
+  </si>
+  <si>
+    <t>As light</t>
+  </si>
+  <si>
+    <t>Agent</t>
   </si>
 </sst>
 </file>
@@ -342,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -703,6 +739,43 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -716,7 +789,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -867,12 +940,99 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -885,96 +1045,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1259,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1281,33 +1365,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="G1" s="56" t="s">
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="G1" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="L1" s="56" t="s">
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="L1" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="G2" s="63" t="s">
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="G2" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -1361,10 +1445,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="62" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="43" t="s">
@@ -1376,10 +1460,10 @@
       <c r="F4" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="62" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="43" t="s">
@@ -1391,10 +1475,10 @@
       <c r="K4" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="54" t="s">
+      <c r="L4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="86" t="s">
         <v>6</v>
       </c>
       <c r="N4" s="12" t="s">
@@ -1412,8 +1496,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="65"/>
-      <c r="C5" s="58"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="43" t="s">
         <v>10</v>
       </c>
@@ -1423,8 +1507,8 @@
       <c r="F5" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="65"/>
-      <c r="H5" s="58"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="62"/>
       <c r="I5" s="43" t="s">
         <v>10</v>
       </c>
@@ -1434,8 +1518,8 @@
       <c r="K5" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="58"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="62"/>
       <c r="N5" s="50" t="s">
         <v>7</v>
       </c>
@@ -1448,8 +1532,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B6" s="65"/>
-      <c r="C6" s="58"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="43" t="s">
         <v>11</v>
       </c>
@@ -1459,8 +1543,8 @@
       <c r="F6" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="65"/>
-      <c r="H6" s="58"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="62"/>
       <c r="I6" s="43" t="s">
         <v>11</v>
       </c>
@@ -1470,8 +1554,8 @@
       <c r="K6" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="54"/>
-      <c r="M6" s="59"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="63"/>
       <c r="N6" s="16" t="s">
         <v>8</v>
       </c>
@@ -1484,8 +1568,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="65"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1495,8 +1579,8 @@
       <c r="F7" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="65"/>
-      <c r="H7" s="59"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="63"/>
       <c r="I7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1506,8 +1590,8 @@
       <c r="K7" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="54"/>
-      <c r="M7" s="60" t="s">
+      <c r="L7" s="83"/>
+      <c r="M7" s="64" t="s">
         <v>7</v>
       </c>
       <c r="N7" s="15" t="s">
@@ -1522,15 +1606,15 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="65"/>
-      <c r="C8" s="60" t="s">
+      <c r="B8" s="60"/>
+      <c r="C8" s="64" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="65"/>
-      <c r="H8" s="60" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="15" t="s">
@@ -1538,8 +1622,8 @@
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="61"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="65"/>
       <c r="N8" s="17" t="s">
         <v>7</v>
       </c>
@@ -1552,20 +1636,20 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="65"/>
-      <c r="C9" s="61"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="65"/>
       <c r="D9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="65"/>
-      <c r="H9" s="61"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="45" t="s">
         <v>10</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="62"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="66"/>
       <c r="N9" s="18" t="s">
         <v>8</v>
       </c>
@@ -1578,20 +1662,20 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="65"/>
-      <c r="C10" s="61"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="65"/>
-      <c r="H10" s="61"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="65"/>
       <c r="I10" s="45" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="57" t="s">
+      <c r="L10" s="83"/>
+      <c r="M10" s="86" t="s">
         <v>8</v>
       </c>
       <c r="N10" s="14" t="s">
@@ -1602,20 +1686,20 @@
       <c r="R10" s="37"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="65"/>
-      <c r="C11" s="62"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="65"/>
-      <c r="H11" s="62"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="66"/>
       <c r="I11" s="18" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="58"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="62"/>
       <c r="N11" s="50" t="s">
         <v>7</v>
       </c>
@@ -1633,8 +1717,8 @@
       <c r="A12" s="7">
         <v>3</v>
       </c>
-      <c r="B12" s="65"/>
-      <c r="C12" s="67" t="s">
+      <c r="B12" s="60"/>
+      <c r="C12" s="77" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="21" t="s">
@@ -1646,8 +1730,8 @@
       <c r="F12" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="65"/>
-      <c r="H12" s="67" t="s">
+      <c r="G12" s="60"/>
+      <c r="H12" s="77" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="21" t="s">
@@ -1659,8 +1743,8 @@
       <c r="K12" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L12" s="54"/>
-      <c r="M12" s="58"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="62"/>
       <c r="N12" s="14" t="s">
         <v>8</v>
       </c>
@@ -1676,8 +1760,8 @@
       <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="68"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="44" t="s">
         <v>10</v>
       </c>
@@ -1687,8 +1771,8 @@
       <c r="F13" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="65"/>
-      <c r="H13" s="68"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="78"/>
       <c r="I13" s="22" t="s">
         <v>10</v>
       </c>
@@ -1698,10 +1782,10 @@
       <c r="K13" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="54" t="s">
+      <c r="L13" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="M13" s="52" t="s">
+      <c r="M13" s="58" t="s">
         <v>6</v>
       </c>
       <c r="N13" s="14" t="s">
@@ -1722,8 +1806,8 @@
       <c r="A14" s="7">
         <v>5</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="68"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="44" t="s">
         <v>11</v>
       </c>
@@ -1733,8 +1817,8 @@
       <c r="F14" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="65"/>
-      <c r="H14" s="68"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="78"/>
       <c r="I14" s="22" t="s">
         <v>11</v>
       </c>
@@ -1744,8 +1828,8 @@
       <c r="K14" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="54"/>
-      <c r="M14" s="52"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="58"/>
       <c r="N14" s="50" t="s">
         <v>7</v>
       </c>
@@ -1761,8 +1845,8 @@
       <c r="A15" s="7">
         <v>2</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="70"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="23" t="s">
         <v>12</v>
       </c>
@@ -1772,8 +1856,8 @@
       <c r="F15" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="71"/>
-      <c r="H15" s="70"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="79"/>
       <c r="I15" s="23" t="s">
         <v>12</v>
       </c>
@@ -1783,8 +1867,8 @@
       <c r="K15" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L15" s="54"/>
-      <c r="M15" s="52"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="58"/>
       <c r="N15" s="14" t="s">
         <v>8</v>
       </c>
@@ -1797,10 +1881,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="62" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="43" t="s">
@@ -1812,10 +1896,10 @@
       <c r="F16" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="64" t="s">
+      <c r="G16" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="58" t="s">
+      <c r="H16" s="62" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="43" t="s">
@@ -1827,8 +1911,8 @@
       <c r="K16" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="54"/>
-      <c r="M16" s="53" t="s">
+      <c r="L16" s="83"/>
+      <c r="M16" s="67" t="s">
         <v>7</v>
       </c>
       <c r="N16" s="17" t="s">
@@ -1845,8 +1929,8 @@
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="65"/>
-      <c r="C17" s="58"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="43" t="s">
         <v>10</v>
       </c>
@@ -1856,8 +1940,8 @@
       <c r="F17" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="65"/>
-      <c r="H17" s="58"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="62"/>
       <c r="I17" s="43" t="s">
         <v>10</v>
       </c>
@@ -1867,8 +1951,8 @@
       <c r="K17" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L17" s="54"/>
-      <c r="M17" s="53"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="67"/>
       <c r="N17" s="17" t="s">
         <v>7</v>
       </c>
@@ -1881,8 +1965,8 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="65"/>
-      <c r="C18" s="58"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="62"/>
       <c r="D18" s="43" t="s">
         <v>11</v>
       </c>
@@ -1892,8 +1976,8 @@
       <c r="F18" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="65"/>
-      <c r="H18" s="58"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="62"/>
       <c r="I18" s="43" t="s">
         <v>11</v>
       </c>
@@ -1903,8 +1987,8 @@
       <c r="K18" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="53"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="67"/>
       <c r="N18" s="17" t="s">
         <v>8</v>
       </c>
@@ -1917,8 +2001,8 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="65"/>
-      <c r="C19" s="59"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="16" t="s">
         <v>12</v>
       </c>
@@ -1928,8 +2012,8 @@
       <c r="F19" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="65"/>
-      <c r="H19" s="59"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="63"/>
       <c r="I19" s="16" t="s">
         <v>12</v>
       </c>
@@ -1939,8 +2023,8 @@
       <c r="K19" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="54"/>
-      <c r="M19" s="52" t="s">
+      <c r="L19" s="83"/>
+      <c r="M19" s="58" t="s">
         <v>8</v>
       </c>
       <c r="N19" s="14" t="s">
@@ -1957,15 +2041,15 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="65"/>
-      <c r="C20" s="60" t="s">
+      <c r="B20" s="60"/>
+      <c r="C20" s="64" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="65"/>
-      <c r="H20" s="60" t="s">
+      <c r="G20" s="60"/>
+      <c r="H20" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I20" s="15" t="s">
@@ -1973,8 +2057,8 @@
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="52"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="58"/>
       <c r="N20" s="50" t="s">
         <v>7</v>
       </c>
@@ -1987,20 +2071,20 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="65"/>
-      <c r="C21" s="61"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="65"/>
-      <c r="H21" s="61"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="65"/>
       <c r="I21" s="45" t="s">
         <v>10</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="52"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="58"/>
       <c r="N21" s="14" t="s">
         <v>8</v>
       </c>
@@ -2013,22 +2097,22 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="65"/>
-      <c r="C22" s="61"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="65"/>
       <c r="D22" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="65"/>
-      <c r="H22" s="61"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="65"/>
       <c r="I22" s="45" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="54" t="s">
+      <c r="L22" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="52" t="s">
+      <c r="M22" s="58" t="s">
         <v>6</v>
       </c>
       <c r="N22" s="14" t="s">
@@ -2046,20 +2130,20 @@
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="65"/>
-      <c r="C23" s="62"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="65"/>
-      <c r="H23" s="62"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="66"/>
       <c r="I23" s="18" t="s">
         <v>12</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="52"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="58"/>
       <c r="N23" s="50" t="s">
         <v>7</v>
       </c>
@@ -2072,8 +2156,8 @@
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="65"/>
-      <c r="C24" s="67" t="s">
+      <c r="B24" s="60"/>
+      <c r="C24" s="77" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -2085,8 +2169,8 @@
       <c r="F24" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="65"/>
-      <c r="H24" s="67" t="s">
+      <c r="G24" s="60"/>
+      <c r="H24" s="77" t="s">
         <v>8</v>
       </c>
       <c r="I24" s="21" t="s">
@@ -2098,8 +2182,8 @@
       <c r="K24" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="54"/>
-      <c r="M24" s="52"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="58"/>
       <c r="N24" s="14" t="s">
         <v>8</v>
       </c>
@@ -2112,8 +2196,8 @@
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="65"/>
-      <c r="C25" s="68"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="78"/>
       <c r="D25" s="44" t="s">
         <v>10</v>
       </c>
@@ -2123,8 +2207,8 @@
       <c r="F25" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="65"/>
-      <c r="H25" s="68"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="78"/>
       <c r="I25" s="22" t="s">
         <v>10</v>
       </c>
@@ -2134,8 +2218,8 @@
       <c r="K25" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L25" s="54"/>
-      <c r="M25" s="53" t="s">
+      <c r="L25" s="83"/>
+      <c r="M25" s="67" t="s">
         <v>7</v>
       </c>
       <c r="N25" s="17" t="s">
@@ -2150,8 +2234,8 @@
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="65"/>
-      <c r="C26" s="68"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="78"/>
       <c r="D26" s="44" t="s">
         <v>11</v>
       </c>
@@ -2161,8 +2245,8 @@
       <c r="F26" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G26" s="65"/>
-      <c r="H26" s="68"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="78"/>
       <c r="I26" s="22" t="s">
         <v>11</v>
       </c>
@@ -2172,8 +2256,8 @@
       <c r="K26" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L26" s="54"/>
-      <c r="M26" s="53"/>
+      <c r="L26" s="83"/>
+      <c r="M26" s="67"/>
       <c r="N26" s="17" t="s">
         <v>7</v>
       </c>
@@ -2186,8 +2270,8 @@
       </c>
     </row>
     <row r="27" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="71"/>
-      <c r="C27" s="70"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="79"/>
       <c r="D27" s="23" t="s">
         <v>12</v>
       </c>
@@ -2197,8 +2281,8 @@
       <c r="F27" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="71"/>
-      <c r="H27" s="70"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="79"/>
       <c r="I27" s="23" t="s">
         <v>12</v>
       </c>
@@ -2208,8 +2292,8 @@
       <c r="K27" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L27" s="54"/>
-      <c r="M27" s="53"/>
+      <c r="L27" s="83"/>
+      <c r="M27" s="67"/>
       <c r="N27" s="17" t="s">
         <v>8</v>
       </c>
@@ -2222,10 +2306,10 @@
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="64" t="s">
+      <c r="B28" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="62" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="43" t="s">
@@ -2237,10 +2321,10 @@
       <c r="F28" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="64" t="s">
+      <c r="G28" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="58" t="s">
+      <c r="H28" s="62" t="s">
         <v>6</v>
       </c>
       <c r="I28" s="43" t="s">
@@ -2252,8 +2336,8 @@
       <c r="K28" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L28" s="54"/>
-      <c r="M28" s="52" t="s">
+      <c r="L28" s="83"/>
+      <c r="M28" s="58" t="s">
         <v>8</v>
       </c>
       <c r="N28" s="14" t="s">
@@ -2261,8 +2345,8 @@
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B29" s="65"/>
-      <c r="C29" s="58"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="62"/>
       <c r="D29" s="43" t="s">
         <v>10</v>
       </c>
@@ -2272,8 +2356,8 @@
       <c r="F29" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="65"/>
-      <c r="H29" s="58"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="62"/>
       <c r="I29" s="43" t="s">
         <v>10</v>
       </c>
@@ -2283,15 +2367,15 @@
       <c r="K29" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L29" s="54"/>
-      <c r="M29" s="52"/>
+      <c r="L29" s="83"/>
+      <c r="M29" s="58"/>
       <c r="N29" s="50" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="65"/>
-      <c r="C30" s="58"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="62"/>
       <c r="D30" s="43" t="s">
         <v>11</v>
       </c>
@@ -2301,8 +2385,8 @@
       <c r="F30" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="65"/>
-      <c r="H30" s="58"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="62"/>
       <c r="I30" s="43" t="s">
         <v>11</v>
       </c>
@@ -2312,15 +2396,15 @@
       <c r="K30" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L30" s="55"/>
-      <c r="M30" s="87"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="59"/>
       <c r="N30" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="65"/>
-      <c r="C31" s="59"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="16" t="s">
         <v>12</v>
       </c>
@@ -2330,8 +2414,8 @@
       <c r="F31" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="65"/>
-      <c r="H31" s="59"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="63"/>
       <c r="I31" s="16" t="s">
         <v>12</v>
       </c>
@@ -2348,15 +2432,15 @@
       <c r="R31" s="11"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="65"/>
-      <c r="C32" s="60" t="s">
+      <c r="B32" s="60"/>
+      <c r="C32" s="64" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="65"/>
-      <c r="H32" s="60" t="s">
+      <c r="G32" s="60"/>
+      <c r="H32" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I32" s="15" t="s">
@@ -2371,13 +2455,13 @@
       <c r="R32" s="13"/>
     </row>
     <row r="33" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="65"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="65"/>
       <c r="D33" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="65"/>
-      <c r="H33" s="61"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="65"/>
       <c r="I33" s="45" t="s">
         <v>10</v>
       </c>
@@ -2392,23 +2476,25 @@
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B34" s="65"/>
-      <c r="C34" s="61"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="65"/>
       <c r="D34" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="61"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="65"/>
       <c r="I34" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="J34" s="7"/>
+      <c r="J34" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="K34" s="7"/>
-      <c r="L34" s="72" t="s">
+      <c r="L34" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M34" s="73"/>
-      <c r="N34" s="74"/>
+      <c r="M34" s="69"/>
+      <c r="N34" s="70"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="3" t="s">
         <v>43</v>
@@ -2418,21 +2504,21 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="65"/>
-      <c r="C35" s="62"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="65"/>
-      <c r="H35" s="62"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="66"/>
       <c r="I35" s="18" t="s">
         <v>12</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="75"/>
-      <c r="M35" s="76"/>
-      <c r="N35" s="77"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="73"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="3" t="s">
         <v>45</v>
@@ -2442,8 +2528,8 @@
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B36" s="65"/>
-      <c r="C36" s="67" t="s">
+      <c r="B36" s="60"/>
+      <c r="C36" s="77" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="21" t="s">
@@ -2455,8 +2541,8 @@
       <c r="F36" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="65"/>
-      <c r="H36" s="67" t="s">
+      <c r="G36" s="60"/>
+      <c r="H36" s="77" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="21" t="s">
@@ -2468,11 +2554,11 @@
       <c r="K36" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L36" s="78" t="s">
+      <c r="L36" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="M36" s="79"/>
-      <c r="N36" s="80"/>
+      <c r="M36" s="75"/>
+      <c r="N36" s="76"/>
       <c r="P36" s="5" t="s">
         <v>40</v>
       </c>
@@ -2480,8 +2566,8 @@
       <c r="R36" s="13"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B37" s="65"/>
-      <c r="C37" s="68"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="78"/>
       <c r="D37" s="22" t="s">
         <v>10</v>
       </c>
@@ -2491,8 +2577,8 @@
       <c r="F37" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="G37" s="65"/>
-      <c r="H37" s="68"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="78"/>
       <c r="I37" s="22" t="s">
         <v>10</v>
       </c>
@@ -2502,9 +2588,9 @@
       <c r="K37" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L37" s="78"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="80"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="76"/>
       <c r="P37" s="5" t="s">
         <v>41</v>
       </c>
@@ -2512,8 +2598,8 @@
       <c r="R37" s="13"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B38" s="65"/>
-      <c r="C38" s="68"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="22" t="s">
         <v>11</v>
       </c>
@@ -2523,8 +2609,8 @@
       <c r="F38" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="65"/>
-      <c r="H38" s="68"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="78"/>
       <c r="I38" s="22" t="s">
         <v>11</v>
       </c>
@@ -2534,11 +2620,11 @@
       <c r="K38" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L38" s="81" t="s">
+      <c r="L38" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="M38" s="82"/>
-      <c r="N38" s="83"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="54"/>
       <c r="P38" s="5" t="s">
         <v>48</v>
       </c>
@@ -2546,8 +2632,8 @@
       <c r="R38" s="13"/>
     </row>
     <row r="39" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="66"/>
-      <c r="C39" s="69"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="82"/>
       <c r="D39" s="24" t="s">
         <v>12</v>
       </c>
@@ -2557,8 +2643,8 @@
       <c r="F39" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="66"/>
-      <c r="H39" s="69"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="82"/>
       <c r="I39" s="24" t="s">
         <v>12</v>
       </c>
@@ -2568,9 +2654,9 @@
       <c r="K39" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L39" s="84"/>
-      <c r="M39" s="85"/>
-      <c r="N39" s="86"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="57"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="19" t="s">
         <v>49</v>
@@ -2592,6 +2678,9 @@
       <c r="K42" s="1"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B43" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="J43" s="1"/>
       <c r="P43" s="42"/>
     </row>
@@ -2606,34 +2695,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="L38:N39"/>
-    <mergeCell ref="M28:M30"/>
-    <mergeCell ref="G4:G15"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="M13:M15"/>
-    <mergeCell ref="M16:M18"/>
-    <mergeCell ref="L34:N35"/>
-    <mergeCell ref="L36:N37"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="B4:B15"/>
-    <mergeCell ref="B16:B27"/>
-    <mergeCell ref="B28:B39"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="H32:H35"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="G16:G27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="H24:H27"/>
     <mergeCell ref="M22:M24"/>
     <mergeCell ref="M25:M27"/>
     <mergeCell ref="L22:L30"/>
@@ -2650,6 +2711,34 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G28:G39"/>
     <mergeCell ref="H28:H31"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="B16:B27"/>
+    <mergeCell ref="B28:B39"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="L38:N39"/>
+    <mergeCell ref="M28:M30"/>
+    <mergeCell ref="G4:G15"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="M13:M15"/>
+    <mergeCell ref="M16:M18"/>
+    <mergeCell ref="L34:N35"/>
+    <mergeCell ref="L36:N37"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="G16:G27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="H24:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2657,4 +2746,232 @@
     <ignoredError sqref="R19" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DAD344-F44B-4DD1-865B-D9B0B9D04C68}">
+  <dimension ref="B1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="98" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E11" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="91">
+        <v>4000</v>
+      </c>
+      <c r="I11" s="92">
+        <v>1000</v>
+      </c>
+      <c r="J11" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="91">
+        <v>10</v>
+      </c>
+      <c r="L11" s="92">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E12" s="90"/>
+      <c r="F12" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="91">
+        <v>4000</v>
+      </c>
+      <c r="I12" s="92">
+        <v>750</v>
+      </c>
+      <c r="J12" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="91">
+        <v>15</v>
+      </c>
+      <c r="L12" s="92">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="F13" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="91">
+        <v>5000</v>
+      </c>
+      <c r="I13" s="92">
+        <v>750</v>
+      </c>
+      <c r="J13" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="91">
+        <v>15</v>
+      </c>
+      <c r="L13" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E14" s="90" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="92" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="91">
+        <v>4000</v>
+      </c>
+      <c r="I14" s="92">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="95">
+        <v>15</v>
+      </c>
+      <c r="L14" s="92">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E15" s="90"/>
+      <c r="F15" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="91">
+        <v>5000</v>
+      </c>
+      <c r="I15" s="92">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="95">
+        <v>15</v>
+      </c>
+      <c r="L15" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="93">
+        <v>5000</v>
+      </c>
+      <c r="I16" s="94">
+        <v>500</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="93">
+        <v>15</v>
+      </c>
+      <c r="L16" s="94">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>